<commit_message>
basic descriptive stats + accompanying figs for pcs complete
</commit_message>
<xml_diff>
--- a/summary_stats.xlsx
+++ b/summary_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m296398\Desktop\medicare_hos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE214E5-5B47-4EFF-98F7-DE4B5C52E6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DAE0C2-D133-4C5F-A7B7-B68FDF0F33D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="315" windowWidth="14730" windowHeight="16155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="demos" sheetId="1" r:id="rId1"/>
@@ -2878,10 +2878,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3078,70 +3078,54 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" s="11">
+        <f>SUM(G3:G7)</f>
+        <v>99.899999999999991</v>
+      </c>
+      <c r="H8" s="11">
+        <f>SUM(H3:H7)</f>
+        <v>99.999999999999986</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B9" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C9" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D9" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E9" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F9" s="19">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G9" s="18">
         <v>21.3</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H9" s="18">
         <v>24.3</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I9" s="18">
         <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>195</v>
-      </c>
-      <c r="C9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" t="s">
-        <v>197</v>
-      </c>
-      <c r="E9" t="s">
-        <v>166</v>
-      </c>
-      <c r="F9" t="s">
-        <v>166</v>
-      </c>
-      <c r="G9">
-        <v>43.4</v>
-      </c>
-      <c r="H9">
-        <v>42.1</v>
-      </c>
-      <c r="I9">
-        <v>-1.3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E10" t="s">
         <v>166</v>
@@ -3150,134 +3134,115 @@
         <v>166</v>
       </c>
       <c r="G10">
+        <v>43.4</v>
+      </c>
+      <c r="H10">
+        <v>42.1</v>
+      </c>
+      <c r="I10">
+        <v>-1.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>198</v>
+      </c>
+      <c r="C11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" t="s">
+        <v>166</v>
+      </c>
+      <c r="F11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G11">
         <v>35.299999999999997</v>
       </c>
-      <c r="H10">
+      <c r="H11">
         <v>33.700000000000003</v>
       </c>
-      <c r="I10">
+      <c r="I11">
         <v>-1.5999999999999901</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="11">
+        <f>SUM(G9:G11)</f>
+        <v>100</v>
+      </c>
+      <c r="H12" s="11">
+        <f>SUM(H9:H11)</f>
+        <v>100.10000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B13" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C13" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D13" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E13" s="21">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F13" s="19">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G13" s="18">
         <v>36.1</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H13" s="18">
         <v>36.299999999999997</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I13" s="18">
         <v>0.19999999999999599</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>195</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>203</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D14" t="s">
         <v>204</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E14" t="s">
         <v>166</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F14" t="s">
         <v>166</v>
       </c>
-      <c r="G12">
+      <c r="G14">
         <v>39.6</v>
       </c>
-      <c r="H12">
+      <c r="H14">
         <v>40.799999999999997</v>
       </c>
-      <c r="I12">
+      <c r="I14">
         <v>1.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>198</v>
-      </c>
-      <c r="C13" t="s">
-        <v>205</v>
-      </c>
-      <c r="D13" t="s">
-        <v>206</v>
-      </c>
-      <c r="E13" t="s">
-        <v>166</v>
-      </c>
-      <c r="F13" t="s">
-        <v>166</v>
-      </c>
-      <c r="G13">
-        <v>24.4</v>
-      </c>
-      <c r="H13">
-        <v>23</v>
-      </c>
-      <c r="I13">
-        <v>-1.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="F14" s="23">
-        <v>0.37</v>
-      </c>
-      <c r="G14" s="18">
-        <v>56.8</v>
-      </c>
-      <c r="H14" s="18">
-        <v>74.099999999999994</v>
-      </c>
-      <c r="I14" s="24">
-        <v>17.3</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="C15" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D15" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E15" t="s">
         <v>166</v>
@@ -3286,160 +3251,128 @@
         <v>166</v>
       </c>
       <c r="G15">
+        <v>24.4</v>
+      </c>
+      <c r="H15">
+        <v>23</v>
+      </c>
+      <c r="I15">
+        <v>-1.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="11">
+        <f>SUM(G13:G15)</f>
+        <v>100.1</v>
+      </c>
+      <c r="H16" s="11">
+        <f>SUM(H13:H15)</f>
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F17" s="23">
+        <v>0.37</v>
+      </c>
+      <c r="G17" s="18">
+        <v>56.8</v>
+      </c>
+      <c r="H17" s="18">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="I17" s="24">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" t="s">
+        <v>212</v>
+      </c>
+      <c r="E18" t="s">
+        <v>166</v>
+      </c>
+      <c r="F18" t="s">
+        <v>166</v>
+      </c>
+      <c r="G18">
         <v>43.2</v>
       </c>
-      <c r="H15">
+      <c r="H18">
         <v>25.9</v>
       </c>
-      <c r="I15">
+      <c r="I18">
         <v>-17.3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G19" s="11">
+        <f>SUM(G17:G18)</f>
+        <v>100</v>
+      </c>
+      <c r="H19" s="11">
+        <f>SUM(H17:H18)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B20" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C20" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D20" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E20" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F20" s="23">
         <v>0.45500000000000002</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G20" s="18">
         <v>54.6</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H20" s="18">
         <v>75.7</v>
       </c>
-      <c r="I16" s="24">
+      <c r="I20" s="24">
         <v>21.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>216</v>
-      </c>
-      <c r="C17" t="s">
-        <v>217</v>
-      </c>
-      <c r="D17" t="s">
-        <v>218</v>
-      </c>
-      <c r="E17" t="s">
-        <v>166</v>
-      </c>
-      <c r="F17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G17">
-        <v>45.4</v>
-      </c>
-      <c r="H17">
-        <v>24.3</v>
-      </c>
-      <c r="I17">
-        <v>-21.1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>239</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="F18" s="23">
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="G18" s="18">
-        <v>2.9</v>
-      </c>
-      <c r="H18" s="18">
-        <v>7</v>
-      </c>
-      <c r="I18" s="18">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>222</v>
-      </c>
-      <c r="C19" t="s">
-        <v>223</v>
-      </c>
-      <c r="D19" t="s">
-        <v>224</v>
-      </c>
-      <c r="E19" t="s">
-        <v>166</v>
-      </c>
-      <c r="F19" t="s">
-        <v>166</v>
-      </c>
-      <c r="G19">
-        <v>18.3</v>
-      </c>
-      <c r="H19">
-        <v>21.8</v>
-      </c>
-      <c r="I19">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>225</v>
-      </c>
-      <c r="C20" t="s">
-        <v>226</v>
-      </c>
-      <c r="D20" t="s">
-        <v>227</v>
-      </c>
-      <c r="E20" t="s">
-        <v>166</v>
-      </c>
-      <c r="F20" t="s">
-        <v>166</v>
-      </c>
-      <c r="G20">
-        <v>28.8</v>
-      </c>
-      <c r="H20">
-        <v>22.1</v>
-      </c>
-      <c r="I20" s="25">
-        <v>-6.7</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="C21" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="D21" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="E21" t="s">
         <v>166</v>
@@ -3448,39 +3381,166 @@
         <v>166</v>
       </c>
       <c r="G21">
+        <v>45.4</v>
+      </c>
+      <c r="H21">
+        <v>24.3</v>
+      </c>
+      <c r="I21">
+        <v>-21.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G22" s="11">
+        <f>SUM(G20:G21)</f>
+        <v>100</v>
+      </c>
+      <c r="H22" s="11">
+        <f>SUM(H20:H21)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F23" s="23">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="G23" s="18">
+        <v>2.9</v>
+      </c>
+      <c r="H23" s="18">
+        <v>7</v>
+      </c>
+      <c r="I23" s="18">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" t="s">
+        <v>223</v>
+      </c>
+      <c r="D24" t="s">
+        <v>224</v>
+      </c>
+      <c r="E24" t="s">
+        <v>166</v>
+      </c>
+      <c r="F24" t="s">
+        <v>166</v>
+      </c>
+      <c r="G24">
+        <v>18.3</v>
+      </c>
+      <c r="H24">
+        <v>21.8</v>
+      </c>
+      <c r="I24">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>225</v>
+      </c>
+      <c r="C25" t="s">
+        <v>226</v>
+      </c>
+      <c r="D25" t="s">
+        <v>227</v>
+      </c>
+      <c r="E25" t="s">
+        <v>166</v>
+      </c>
+      <c r="F25" t="s">
+        <v>166</v>
+      </c>
+      <c r="G25">
+        <v>28.8</v>
+      </c>
+      <c r="H25">
+        <v>22.1</v>
+      </c>
+      <c r="I25" s="25">
+        <v>-6.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>228</v>
+      </c>
+      <c r="C26" t="s">
+        <v>229</v>
+      </c>
+      <c r="D26" t="s">
+        <v>230</v>
+      </c>
+      <c r="E26" t="s">
+        <v>166</v>
+      </c>
+      <c r="F26" t="s">
+        <v>166</v>
+      </c>
+      <c r="G26">
         <v>26.7</v>
       </c>
-      <c r="H21">
+      <c r="H26">
         <v>32.5</v>
       </c>
-      <c r="I21">
+      <c r="I26">
         <v>5.8</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>231</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C27" t="s">
         <v>232</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D27" t="s">
         <v>233</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E27" t="s">
         <v>166</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F27" t="s">
         <v>166</v>
       </c>
-      <c r="G22">
+      <c r="G27">
         <v>23.2</v>
       </c>
-      <c r="H22">
+      <c r="H27">
         <v>16.600000000000001</v>
       </c>
-      <c r="I22" s="25">
+      <c r="I27" s="25">
         <v>-6.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G28" s="11">
+        <f>SUM(G23:G27)</f>
+        <v>99.9</v>
+      </c>
+      <c r="H28" s="11">
+        <f>SUM(H23:H27)</f>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mcs descriptives + figs (basic) completed
</commit_message>
<xml_diff>
--- a/summary_stats.xlsx
+++ b/summary_stats.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m296398\Desktop\medicare_hos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DAE0C2-D133-4C5F-A7B7-B68FDF0F33D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E78F0DB-CDD0-4EB0-94DD-50943DDEFCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="315" windowWidth="14730" windowHeight="16155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="315" windowWidth="14730" windowHeight="16155" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="demos" sheetId="1" r:id="rId1"/>
     <sheet name="comorb" sheetId="2" r:id="rId2"/>
     <sheet name="pcs" sheetId="3" r:id="rId3"/>
+    <sheet name="mcs" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="320">
   <si>
     <t>NA</t>
   </si>
@@ -535,6 +536,228 @@
     <t>24526 (41.5)</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>Cohort 1 (1998)</t>
+  </si>
+  <si>
+    <t>Cohort 23 (2020)</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>Cohort1_percent</t>
+  </si>
+  <si>
+    <t>Cohort2_percent</t>
+  </si>
+  <si>
+    <t>percent_diff</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Poor</t>
+  </si>
+  <si>
+    <t>479 (4.1)</t>
+  </si>
+  <si>
+    <t>3062 (5.2)</t>
+  </si>
+  <si>
+    <t>&lt;0.001</t>
+  </si>
+  <si>
+    <t>Fair</t>
+  </si>
+  <si>
+    <t>3108 (26.8)</t>
+  </si>
+  <si>
+    <t>14913 (25.2)</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>5249 (45.2)</t>
+  </si>
+  <si>
+    <t>24316 (41.2)</t>
+  </si>
+  <si>
+    <t>Very Good</t>
+  </si>
+  <si>
+    <t>2404 (20.7)</t>
+  </si>
+  <si>
+    <t>14369 (24.3)</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>363 (3.1)</t>
+  </si>
+  <si>
+    <t>2430 (4.1)</t>
+  </si>
+  <si>
+    <t>Yes, limited a lot</t>
+  </si>
+  <si>
+    <t>2467 (21.3)</t>
+  </si>
+  <si>
+    <t>14335 (24.3)</t>
+  </si>
+  <si>
+    <t>Yes, limited a little</t>
+  </si>
+  <si>
+    <t>5040 (43.4)</t>
+  </si>
+  <si>
+    <t>24857 (42.1)</t>
+  </si>
+  <si>
+    <t>No, not limited at all</t>
+  </si>
+  <si>
+    <t>4096 (35.3)</t>
+  </si>
+  <si>
+    <t>19898 (33.7)</t>
+  </si>
+  <si>
+    <t>4185 (36.1)</t>
+  </si>
+  <si>
+    <t>21422 (36.3)</t>
+  </si>
+  <si>
+    <t>4592 (39.6)</t>
+  </si>
+  <si>
+    <t>24080 (40.8)</t>
+  </si>
+  <si>
+    <t>2826 (24.4)</t>
+  </si>
+  <si>
+    <t>13588 (23.0)</t>
+  </si>
+  <si>
+    <t>Yes, accomplished less</t>
+  </si>
+  <si>
+    <t>6593 (56.8)</t>
+  </si>
+  <si>
+    <t>43797 (74.1)</t>
+  </si>
+  <si>
+    <t>No, not affected</t>
+  </si>
+  <si>
+    <t>5010 (43.2)</t>
+  </si>
+  <si>
+    <t>15293 (25.9)</t>
+  </si>
+  <si>
+    <t>Yes, limited</t>
+  </si>
+  <si>
+    <t>6332 (54.6)</t>
+  </si>
+  <si>
+    <t>44734 (75.7)</t>
+  </si>
+  <si>
+    <t>No, not limited</t>
+  </si>
+  <si>
+    <t>5271 (45.4)</t>
+  </si>
+  <si>
+    <t>14356 (24.3)</t>
+  </si>
+  <si>
+    <t>Extremely</t>
+  </si>
+  <si>
+    <t>342 (2.9)</t>
+  </si>
+  <si>
+    <t>4154 (7.0)</t>
+  </si>
+  <si>
+    <t>Quite a bit</t>
+  </si>
+  <si>
+    <t>2121 (18.3)</t>
+  </si>
+  <si>
+    <t>12891 (21.8)</t>
+  </si>
+  <si>
+    <t>Moderately</t>
+  </si>
+  <si>
+    <t>3345 (28.8)</t>
+  </si>
+  <si>
+    <t>13052 (22.1)</t>
+  </si>
+  <si>
+    <t>A little bit</t>
+  </si>
+  <si>
+    <t>3100 (26.7)</t>
+  </si>
+  <si>
+    <t>19200 (32.5)</t>
+  </si>
+  <si>
+    <t>Not at all</t>
+  </si>
+  <si>
+    <t>2695 (23.2)</t>
+  </si>
+  <si>
+    <t>9793 (16.6)</t>
+  </si>
+  <si>
+    <t>General_Health (%)</t>
+  </si>
+  <si>
+    <t>Mod_Activity (%)</t>
+  </si>
+  <si>
+    <t>Stairs (%)</t>
+  </si>
+  <si>
+    <t>Phys_Amount_Limit (%)</t>
+  </si>
+  <si>
+    <t>Phys_Type_Limit (%)</t>
+  </si>
+  <si>
+    <t>Pain_Work (%)</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -565,196 +788,214 @@
     <t>n</t>
   </si>
   <si>
-    <t>Poor</t>
-  </si>
-  <si>
-    <t>479 (4.1)</t>
-  </si>
-  <si>
-    <t>3062 (5.2)</t>
+    <t>Yes, accomplished less</t>
+  </si>
+  <si>
+    <t>3744 (32.3)</t>
+  </si>
+  <si>
+    <t>22724 (38.5)</t>
   </si>
   <si>
     <t>&lt;0.001</t>
   </si>
   <si>
-    <t>Fair</t>
-  </si>
-  <si>
-    <t>3108 (26.8)</t>
-  </si>
-  <si>
-    <t>14913 (25.2)</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>5249 (45.2)</t>
-  </si>
-  <si>
-    <t>24316 (41.2)</t>
-  </si>
-  <si>
-    <t>Very Good</t>
-  </si>
-  <si>
-    <t>2404 (20.7)</t>
-  </si>
-  <si>
-    <t>14369 (24.3)</t>
-  </si>
-  <si>
-    <t>Excellent</t>
-  </si>
-  <si>
-    <t>363 (3.1)</t>
-  </si>
-  <si>
-    <t>2430 (4.1)</t>
-  </si>
-  <si>
-    <t>Yes, limited a lot</t>
-  </si>
-  <si>
-    <t>2467 (21.3)</t>
-  </si>
-  <si>
-    <t>14335 (24.3)</t>
-  </si>
-  <si>
-    <t>Yes, limited a little</t>
-  </si>
-  <si>
-    <t>5040 (43.4)</t>
-  </si>
-  <si>
-    <t>24857 (42.1)</t>
-  </si>
-  <si>
-    <t>No, not limited at all</t>
-  </si>
-  <si>
-    <t>4096 (35.3)</t>
-  </si>
-  <si>
-    <t>19898 (33.7)</t>
-  </si>
-  <si>
-    <t>4185 (36.1)</t>
-  </si>
-  <si>
-    <t>21422 (36.3)</t>
-  </si>
-  <si>
-    <t>4592 (39.6)</t>
-  </si>
-  <si>
-    <t>24080 (40.8)</t>
-  </si>
-  <si>
-    <t>2826 (24.4)</t>
-  </si>
-  <si>
-    <t>13588 (23.0)</t>
-  </si>
-  <si>
-    <t>Yes, accomplished less</t>
-  </si>
-  <si>
-    <t>6593 (56.8)</t>
-  </si>
-  <si>
-    <t>43797 (74.1)</t>
-  </si>
-  <si>
     <t>No, not affected</t>
   </si>
   <si>
-    <t>5010 (43.2)</t>
-  </si>
-  <si>
-    <t>15293 (25.9)</t>
-  </si>
-  <si>
-    <t>Yes, limited</t>
-  </si>
-  <si>
-    <t>6332 (54.6)</t>
-  </si>
-  <si>
-    <t>44734 (75.7)</t>
-  </si>
-  <si>
-    <t>No, not limited</t>
-  </si>
-  <si>
-    <t>5271 (45.4)</t>
-  </si>
-  <si>
-    <t>14356 (24.3)</t>
-  </si>
-  <si>
-    <t>Extremely</t>
-  </si>
-  <si>
-    <t>342 (2.9)</t>
-  </si>
-  <si>
-    <t>4154 (7.0)</t>
-  </si>
-  <si>
-    <t>Quite a bit</t>
-  </si>
-  <si>
-    <t>2121 (18.3)</t>
-  </si>
-  <si>
-    <t>12891 (21.8)</t>
-  </si>
-  <si>
-    <t>Moderately</t>
-  </si>
-  <si>
-    <t>3345 (28.8)</t>
-  </si>
-  <si>
-    <t>13052 (22.1)</t>
-  </si>
-  <si>
-    <t>A little bit</t>
-  </si>
-  <si>
-    <t>3100 (26.7)</t>
-  </si>
-  <si>
-    <t>19200 (32.5)</t>
-  </si>
-  <si>
-    <t>Not at all</t>
-  </si>
-  <si>
-    <t>2695 (23.2)</t>
-  </si>
-  <si>
-    <t>9793 (16.6)</t>
-  </si>
-  <si>
-    <t>General_Health (%)</t>
-  </si>
-  <si>
-    <t>Mod_Activity (%)</t>
-  </si>
-  <si>
-    <t>Stairs (%)</t>
-  </si>
-  <si>
-    <t>Phys_Amount_Limit (%)</t>
-  </si>
-  <si>
-    <t>Phys_Type_Limit (%)</t>
-  </si>
-  <si>
-    <t>Pain_Work (%)</t>
+    <t>7859 (67.7)</t>
+  </si>
+  <si>
+    <t>36366 (61.5)</t>
+  </si>
+  <si>
+    <t>Yes, less careful</t>
+  </si>
+  <si>
+    <t>2618 (22.6)</t>
+  </si>
+  <si>
+    <t>18379 (31.1)</t>
+  </si>
+  <si>
+    <t>8985 (77.4)</t>
+  </si>
+  <si>
+    <t>40711 (68.9)</t>
+  </si>
+  <si>
+    <t>None of the time</t>
+  </si>
+  <si>
+    <t>503 (4.3)</t>
+  </si>
+  <si>
+    <t>1005 (1.7)</t>
+  </si>
+  <si>
+    <t>A little of the time</t>
+  </si>
+  <si>
+    <t>1086 (9.4)</t>
+  </si>
+  <si>
+    <t>4263 (7.2)</t>
+  </si>
+  <si>
+    <t>Some of the time</t>
+  </si>
+  <si>
+    <t>2240 (19.3)</t>
+  </si>
+  <si>
+    <t>11109 (18.8)</t>
+  </si>
+  <si>
+    <t>A good bit of the time</t>
+  </si>
+  <si>
+    <t>2022 (17.4)</t>
+  </si>
+  <si>
+    <t>10601 (17.9)</t>
+  </si>
+  <si>
+    <t>Most of the time</t>
+  </si>
+  <si>
+    <t>4565 (39.3)</t>
+  </si>
+  <si>
+    <t>25444 (43.1)</t>
+  </si>
+  <si>
+    <t>All of the time</t>
+  </si>
+  <si>
+    <t>1187 (10.2)</t>
+  </si>
+  <si>
+    <t>6668 (11.3)</t>
+  </si>
+  <si>
+    <t>1367 (11.8)</t>
+  </si>
+  <si>
+    <t>3773 (6.4)</t>
+  </si>
+  <si>
+    <t>2169 (18.7)</t>
+  </si>
+  <si>
+    <t>9618 (16.3)</t>
+  </si>
+  <si>
+    <t>3365 (29.0)</t>
+  </si>
+  <si>
+    <t>16390 (27.7)</t>
+  </si>
+  <si>
+    <t>2172 (18.7)</t>
+  </si>
+  <si>
+    <t>11542 (19.5)</t>
+  </si>
+  <si>
+    <t>2210 (19.0)</t>
+  </si>
+  <si>
+    <t>15894 (26.9)</t>
+  </si>
+  <si>
+    <t>320 (2.8)</t>
+  </si>
+  <si>
+    <t>1873 (3.2)</t>
+  </si>
+  <si>
+    <t>5332 (46.0)</t>
+  </si>
+  <si>
+    <t>21444 (36.3)</t>
+  </si>
+  <si>
+    <t>3360 (29.0)</t>
+  </si>
+  <si>
+    <t>18951 (32.1)</t>
+  </si>
+  <si>
+    <t>2089 (18.0)</t>
+  </si>
+  <si>
+    <t>12209 (20.7)</t>
+  </si>
+  <si>
+    <t>466 (4.0)</t>
+  </si>
+  <si>
+    <t>3494 (5.9)</t>
+  </si>
+  <si>
+    <t>250 (2.2)</t>
+  </si>
+  <si>
+    <t>2180 (3.7)</t>
+  </si>
+  <si>
+    <t>106 (0.9)</t>
+  </si>
+  <si>
+    <t>812 (1.4)</t>
+  </si>
+  <si>
+    <t>5853 (50.4)</t>
+  </si>
+  <si>
+    <t>27962 (47.3)</t>
+  </si>
+  <si>
+    <t>2322 (20.0)</t>
+  </si>
+  <si>
+    <t>10590 (17.9)</t>
+  </si>
+  <si>
+    <t>2398 (20.7)</t>
+  </si>
+  <si>
+    <t>11533 (19.5)</t>
+  </si>
+  <si>
+    <t>786 (6.8)</t>
+  </si>
+  <si>
+    <t>5934 (10.0)</t>
+  </si>
+  <si>
+    <t>244 (2.1)</t>
+  </si>
+  <si>
+    <t>3071 (5.2)</t>
+  </si>
+  <si>
+    <t>Emo_Amount_Limit (%)</t>
+  </si>
+  <si>
+    <t>Emo_Carefulness (%)</t>
+  </si>
+  <si>
+    <t>Peace (%)</t>
+  </si>
+  <si>
+    <t>Energy  (%)</t>
+  </si>
+  <si>
+    <t>Down (%)</t>
+  </si>
+  <si>
+    <t>Social_Interference (%)</t>
   </si>
 </sst>
 </file>
@@ -792,6 +1033,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -805,12 +1052,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -876,19 +1117,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -896,13 +1137,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1412,7 +1651,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1441,7 +1680,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
@@ -1453,34 +1692,34 @@
       <c r="D2">
         <v>59090</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="10">
         <v>0.157</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="10">
         <v>61.7</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="10">
         <v>61</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="10">
         <v>-0.70000000000000295</v>
       </c>
     </row>
@@ -1505,41 +1744,41 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G5" s="11">
+      <c r="G5" s="3">
         <f>SUM(G3:G4)</f>
         <v>100</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="3">
         <f>SUM(H3:H4)</f>
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="11">
         <v>0.28799999999999998</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="10">
         <v>91.3</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="10">
         <v>81.599999999999994</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="4">
         <v>-9.6999999999999993</v>
       </c>
     </row>
@@ -1584,41 +1823,41 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G9" s="11">
+      <c r="G9" s="3">
         <f>SUM(G6:G8)</f>
         <v>100</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="3">
         <f>SUM(H6:H8)</f>
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="11">
         <v>0.218</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="10">
         <v>45.9</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="10">
         <v>35.200000000000003</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="4">
         <v>-10.7</v>
       </c>
     </row>
@@ -1643,41 +1882,41 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G12" s="11">
+      <c r="G12" s="3">
         <f>SUM(G10:G11)</f>
         <v>100</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="3">
         <f>SUM(H10:H11)</f>
         <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="11">
         <v>0.249</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="10">
         <v>59.4</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="10">
         <v>47.1</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="4">
         <v>-12.3</v>
       </c>
     </row>
@@ -1702,41 +1941,41 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G15" s="11">
+      <c r="G15" s="3">
         <f>SUM(G13:G14)</f>
         <v>100</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="3">
         <f>SUM(H13:H14)</f>
         <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="2">
         <v>0.436</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="10">
         <v>26.6</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="10">
         <v>12.7</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="10">
         <v>-13.9</v>
       </c>
     </row>
@@ -1776,46 +2015,46 @@
       <c r="H18">
         <v>55.7</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="5">
         <v>18.8</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G19" s="11">
+      <c r="G19" s="3">
         <f>SUM(G16:G18)</f>
         <v>100</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="3">
         <f>SUM(H16:H18)</f>
         <v>100.1</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="2">
         <v>0.41599999999999998</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="10">
         <v>5</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="10">
         <v>8.9</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="10">
         <v>3.9</v>
       </c>
     </row>
@@ -1895,7 +2134,7 @@
       <c r="H24">
         <v>23.8</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="5">
         <v>10.6</v>
       </c>
     </row>
@@ -1975,7 +2214,7 @@
       <c r="H28">
         <v>9.6999999999999993</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="5">
         <v>-10.1</v>
       </c>
     </row>
@@ -2000,15 +2239,15 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G30" s="11">
+      <c r="G30" s="3">
         <f>SUM(G20:G29)</f>
         <v>99.9</v>
       </c>
-      <c r="H30" s="11">
+      <c r="H30" s="3">
         <f>SUM(H20:H29)</f>
         <v>100.1</v>
       </c>
-      <c r="I30" s="11"/>
+      <c r="I30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2035,7 +2274,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2064,7 +2303,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>92</v>
       </c>
       <c r="B2" t="s">
@@ -2079,36 +2318,36 @@
       <c r="E2" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="10" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="10">
         <v>2.7E-2</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="10">
         <v>2.3E-2</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="10">
         <v>57.4</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="10">
         <v>58.5</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="10">
         <v>-1.1000000000000001</v>
       </c>
     </row>
@@ -2133,41 +2372,41 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G5" s="11">
+      <c r="G5" s="3">
         <f>SUM(G3:G4)</f>
         <v>100</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="3">
         <f>SUM(H3:H4)</f>
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="2">
         <v>0.32600000000000001</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="10">
         <v>56.6</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="10">
         <v>72</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="4">
         <v>15.4</v>
       </c>
     </row>
@@ -2192,41 +2431,41 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G8" s="11">
+      <c r="G8" s="3">
         <f>SUM(G6:G7)</f>
         <v>100</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="3">
         <f>SUM(H6:H7)</f>
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="11">
         <v>0.123</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="10">
         <v>18.7</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="10">
         <v>14.2</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="10">
         <v>-4.5</v>
       </c>
     </row>
@@ -2251,41 +2490,41 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G11" s="11">
+      <c r="G11" s="3">
         <f>SUM(G9:G10)</f>
         <v>100</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="3">
         <f>SUM(H9:H10)</f>
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="10">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="10">
         <v>7.3</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="10">
         <v>9.6</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="10">
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -2310,41 +2549,41 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G14" s="11">
+      <c r="G14" s="3">
         <f>SUM(G12:G13)</f>
         <v>100</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="3">
         <f>SUM(H12:H13)</f>
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="11">
         <v>0.1</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="10">
         <v>11.8</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="10">
         <v>8.8000000000000007</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="10">
         <v>-3</v>
       </c>
     </row>
@@ -2369,41 +2608,41 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G17" s="11">
+      <c r="G17" s="3">
         <f>SUM(G15:G16)</f>
         <v>100</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="3">
         <f>SUM(H15:H16)</f>
         <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="10">
         <v>0.05</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="10">
         <v>23</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="10">
         <v>25.2</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="10">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -2428,41 +2667,41 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G20" s="11">
+      <c r="G20" s="3">
         <f>SUM(G18:G19)</f>
         <v>100</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="3">
         <f>SUM(H18:H19)</f>
         <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="10">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="10">
         <v>6.4</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="10">
         <v>7.6</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="10">
         <v>1.2</v>
       </c>
     </row>
@@ -2487,41 +2726,41 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G23" s="11">
+      <c r="G23" s="3">
         <f>SUM(G21:G22)</f>
         <v>100</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="3">
         <f>SUM(H21:H22)</f>
         <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="11">
         <v>0.18099999999999999</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="10">
         <v>16.3</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H24" s="10">
         <v>23.5</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="4">
         <v>7.2</v>
       </c>
     </row>
@@ -2546,41 +2785,41 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G26" s="11">
+      <c r="G26" s="3">
         <f>SUM(G24:G25)</f>
         <v>100</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="3">
         <f>SUM(H24:H25)</f>
         <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="10">
         <v>0.95599999999999996</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="10">
         <v>1E-3</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="10">
         <v>6.9</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="10">
         <v>6.9</v>
       </c>
-      <c r="I27" s="8">
+      <c r="I27" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2605,41 +2844,41 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G29" s="11">
+      <c r="G29" s="3">
         <f>SUM(G27:G28)</f>
         <v>100</v>
       </c>
-      <c r="H29" s="11">
+      <c r="H29" s="3">
         <f>SUM(H27:H28)</f>
         <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="10">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="10">
         <v>36</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30" s="10">
         <v>38.299999999999997</v>
       </c>
-      <c r="I30" s="8">
+      <c r="I30" s="10">
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -2664,41 +2903,41 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G32" s="11">
+      <c r="G32" s="3">
         <f>SUM(G30:G31)</f>
         <v>100</v>
       </c>
-      <c r="H32" s="11">
+      <c r="H32" s="3">
         <f>SUM(H30:H31)</f>
         <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="10">
+      <c r="F33" s="2">
         <v>0.30399999999999999</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="10">
         <v>17.5</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H33" s="10">
         <v>30.3</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="4">
         <v>12.8</v>
       </c>
     </row>
@@ -2723,41 +2962,41 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G35" s="11">
+      <c r="G35" s="3">
         <f>SUM(G33:G34)</f>
         <v>100</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H35" s="3">
         <f>SUM(H33:H34)</f>
         <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F36" s="10">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="10">
         <v>14.7</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H36" s="10">
         <v>17.2</v>
       </c>
-      <c r="I36" s="8">
+      <c r="I36" s="10">
         <v>2.5</v>
       </c>
     </row>
@@ -2782,41 +3021,41 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G38" s="11">
+      <c r="G38" s="3">
         <f>SUM(G36:G37)</f>
         <v>100</v>
       </c>
-      <c r="H38" s="11">
+      <c r="H38" s="3">
         <f>SUM(H36:H37)</f>
         <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F39" s="10">
+      <c r="F39" s="2">
         <v>0.23499999999999999</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G39" s="10">
         <v>82.9</v>
       </c>
-      <c r="H39" s="8">
+      <c r="H39" s="10">
         <v>90.2</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I39" s="4">
         <v>7.3</v>
       </c>
     </row>
@@ -2856,16 +3095,16 @@
       <c r="H41">
         <v>6.5</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41" s="5">
         <v>-6.9</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G42" s="11">
+      <c r="G42" s="3">
         <f>SUM(G39:G41)</f>
         <v>100.00000000000001</v>
       </c>
-      <c r="H42" s="11">
+      <c r="H42" s="3">
         <f>SUM(H39:H41)</f>
         <v>100</v>
       </c>
@@ -2880,57 +3119,646 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="12">
+        <v>11603</v>
+      </c>
+      <c r="D2" s="12">
+        <v>59090</v>
+      </c>
+      <c r="E2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0.125</v>
+      </c>
+      <c r="G3" s="10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H3" s="10">
+        <v>5.2</v>
+      </c>
+      <c r="I3" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G4">
+        <v>26.8</v>
+      </c>
+      <c r="H4">
+        <v>25.2</v>
+      </c>
+      <c r="I4">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G5">
+        <v>45.2</v>
+      </c>
+      <c r="H5">
+        <v>41.2</v>
+      </c>
+      <c r="I5">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" t="s">
+        <v>188</v>
+      </c>
+      <c r="G6">
+        <v>20.7</v>
+      </c>
+      <c r="H6">
+        <v>24.3</v>
+      </c>
+      <c r="I6">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D7" t="s">
+        <v>191</v>
+      </c>
+      <c r="G7">
+        <v>3.1</v>
+      </c>
+      <c r="H7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" s="3">
+        <f>SUM(G3:G7)</f>
+        <v>99.899999999999991</v>
+      </c>
+      <c r="H8" s="3">
+        <f>SUM(H3:H7)</f>
+        <v>99.999999999999986</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="F9" s="10">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="G9" s="10">
+        <v>21.3</v>
+      </c>
+      <c r="H9" s="10">
+        <v>24.3</v>
+      </c>
+      <c r="I9" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" t="s">
+        <v>197</v>
+      </c>
+      <c r="G10">
+        <v>43.4</v>
+      </c>
+      <c r="H10">
+        <v>42.1</v>
+      </c>
+      <c r="I10">
+        <v>-1.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>198</v>
+      </c>
+      <c r="C11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" t="s">
+        <v>200</v>
+      </c>
+      <c r="G11">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="H11">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="I11">
+        <v>-1.5999999999999901</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="3">
+        <f>SUM(G9:G11)</f>
+        <v>100</v>
+      </c>
+      <c r="H12" s="3">
+        <f>SUM(H9:H11)</f>
+        <v>100.10000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="E13" s="6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F13" s="10">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="G13" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="H13" s="10">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0.19999999999999599</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" t="s">
+        <v>203</v>
+      </c>
+      <c r="D14" t="s">
+        <v>204</v>
+      </c>
+      <c r="G14">
+        <v>39.6</v>
+      </c>
+      <c r="H14">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="I14">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C15" t="s">
+        <v>205</v>
+      </c>
+      <c r="D15" t="s">
+        <v>206</v>
+      </c>
+      <c r="G15">
+        <v>24.4</v>
+      </c>
+      <c r="H15">
+        <v>23</v>
+      </c>
+      <c r="I15">
+        <v>-1.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="3">
+        <f>SUM(G13:G15)</f>
+        <v>100.1</v>
+      </c>
+      <c r="H16" s="3">
+        <f>SUM(H13:H15)</f>
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="G17" s="10">
+        <v>56.8</v>
+      </c>
+      <c r="H17" s="10">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="I17" s="4">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" t="s">
+        <v>212</v>
+      </c>
+      <c r="G18">
+        <v>43.2</v>
+      </c>
+      <c r="H18">
+        <v>25.9</v>
+      </c>
+      <c r="I18">
+        <v>-17.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G19" s="3">
+        <f>SUM(G17:G18)</f>
+        <v>100</v>
+      </c>
+      <c r="H19" s="3">
+        <f>SUM(H17:H18)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="G20" s="10">
+        <v>54.6</v>
+      </c>
+      <c r="H20" s="10">
+        <v>75.7</v>
+      </c>
+      <c r="I20" s="4">
+        <v>21.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C21" t="s">
+        <v>217</v>
+      </c>
+      <c r="D21" t="s">
+        <v>218</v>
+      </c>
+      <c r="G21">
+        <v>45.4</v>
+      </c>
+      <c r="H21">
+        <v>24.3</v>
+      </c>
+      <c r="I21">
+        <v>-21.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G22" s="3">
+        <f>SUM(G20:G21)</f>
+        <v>100</v>
+      </c>
+      <c r="H22" s="3">
+        <f>SUM(H20:H21)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="G23" s="10">
+        <v>2.9</v>
+      </c>
+      <c r="H23" s="10">
+        <v>7</v>
+      </c>
+      <c r="I23" s="10">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" t="s">
+        <v>223</v>
+      </c>
+      <c r="D24" t="s">
+        <v>224</v>
+      </c>
+      <c r="G24">
+        <v>18.3</v>
+      </c>
+      <c r="H24">
+        <v>21.8</v>
+      </c>
+      <c r="I24">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>225</v>
+      </c>
+      <c r="C25" t="s">
+        <v>226</v>
+      </c>
+      <c r="D25" t="s">
+        <v>227</v>
+      </c>
+      <c r="G25">
+        <v>28.8</v>
+      </c>
+      <c r="H25">
+        <v>22.1</v>
+      </c>
+      <c r="I25" s="5">
+        <v>-6.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>228</v>
+      </c>
+      <c r="C26" t="s">
+        <v>229</v>
+      </c>
+      <c r="D26" t="s">
+        <v>230</v>
+      </c>
+      <c r="G26">
+        <v>26.7</v>
+      </c>
+      <c r="H26">
+        <v>32.5</v>
+      </c>
+      <c r="I26">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>231</v>
+      </c>
+      <c r="C27" t="s">
+        <v>232</v>
+      </c>
+      <c r="D27" t="s">
+        <v>233</v>
+      </c>
+      <c r="G27">
+        <v>23.2</v>
+      </c>
+      <c r="H27">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="I27" s="5">
+        <v>-6.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G28" s="3">
+        <f>SUM(G23:G27)</f>
+        <v>99.9</v>
+      </c>
+      <c r="H28" s="3">
+        <f>SUM(H23:H27)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:I35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
     <col min="7" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>167</v>
+        <v>241</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>168</v>
+        <v>242</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>169</v>
+        <v>243</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>170</v>
+        <v>244</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>171</v>
+        <v>245</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>172</v>
+        <v>246</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>173</v>
+        <v>247</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>174</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>175</v>
+        <v>249</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="C2" s="13">
         <v>11603</v>
@@ -2939,608 +3767,790 @@
         <v>59090</v>
       </c>
       <c r="E2" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="F2" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>234</v>
+        <v>314</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>176</v>
+        <v>250</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>177</v>
+        <v>251</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="F3" s="22">
-        <v>0.125</v>
+        <v>252</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="F3" s="20">
+        <v>0.13</v>
       </c>
       <c r="G3" s="18">
-        <v>4.0999999999999996</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="H3" s="18">
-        <v>5.2</v>
-      </c>
-      <c r="I3" s="18">
-        <v>1.1000000000000001</v>
+        <v>38.5</v>
+      </c>
+      <c r="I3" s="22">
+        <v>6.2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>180</v>
+        <v>254</v>
       </c>
       <c r="C4" t="s">
-        <v>181</v>
+        <v>255</v>
       </c>
       <c r="D4" t="s">
-        <v>182</v>
+        <v>256</v>
       </c>
       <c r="E4" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="F4" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="G4">
-        <v>26.8</v>
+        <v>67.7</v>
       </c>
       <c r="H4">
-        <v>25.2</v>
+        <v>61.5</v>
       </c>
       <c r="I4">
-        <v>-1.6</v>
+        <v>-6.2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C5" t="s">
-        <v>184</v>
-      </c>
-      <c r="D5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F5" t="s">
-        <v>166</v>
-      </c>
-      <c r="G5">
-        <v>45.2</v>
-      </c>
-      <c r="H5">
-        <v>41.2</v>
-      </c>
-      <c r="I5">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D6" t="s">
-        <v>188</v>
-      </c>
-      <c r="E6" t="s">
-        <v>166</v>
-      </c>
-      <c r="F6" t="s">
-        <v>166</v>
-      </c>
-      <c r="G6">
-        <v>20.7</v>
-      </c>
-      <c r="H6">
-        <v>24.3</v>
-      </c>
-      <c r="I6">
-        <v>3.6</v>
+      <c r="G5" s="3">
+        <f>SUM(G3:G4)</f>
+        <v>100</v>
+      </c>
+      <c r="H5" s="3">
+        <f>SUM(H3:H4)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="F6" s="20">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="G6" s="18">
+        <v>22.6</v>
+      </c>
+      <c r="H6" s="18">
+        <v>31.1</v>
+      </c>
+      <c r="I6" s="22">
+        <v>8.5</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>189</v>
+        <v>254</v>
       </c>
       <c r="C7" t="s">
-        <v>190</v>
+        <v>260</v>
       </c>
       <c r="D7" t="s">
-        <v>191</v>
+        <v>261</v>
       </c>
       <c r="E7" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="F7" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="G7">
-        <v>3.1</v>
+        <v>77.400000000000006</v>
       </c>
       <c r="H7">
-        <v>4.0999999999999996</v>
+        <v>68.900000000000006</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>-8.5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G8" s="11">
-        <f>SUM(G3:G7)</f>
-        <v>99.899999999999991</v>
-      </c>
-      <c r="H8" s="11">
-        <f>SUM(H3:H7)</f>
-        <v>99.999999999999986</v>
+      <c r="G8" s="3">
+        <f>SUM(G6:G7)</f>
+        <v>100</v>
+      </c>
+      <c r="H8" s="3">
+        <f>SUM(H6:H7)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>235</v>
+        <v>316</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>192</v>
+        <v>262</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>193</v>
+        <v>263</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="F9" s="19">
-        <v>7.1999999999999995E-2</v>
+        <v>264</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="F9" s="20">
+        <v>0.183</v>
       </c>
       <c r="G9" s="18">
-        <v>21.3</v>
+        <v>4.3</v>
       </c>
       <c r="H9" s="18">
-        <v>24.3</v>
-      </c>
-      <c r="I9" s="18">
-        <v>3</v>
+        <v>1.7</v>
+      </c>
+      <c r="I9" s="22">
+        <v>-2.6</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>195</v>
+        <v>265</v>
       </c>
       <c r="C10" t="s">
-        <v>196</v>
+        <v>266</v>
       </c>
       <c r="D10" t="s">
-        <v>197</v>
+        <v>267</v>
       </c>
       <c r="E10" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="F10" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="G10">
-        <v>43.4</v>
+        <v>9.4</v>
       </c>
       <c r="H10">
-        <v>42.1</v>
-      </c>
-      <c r="I10">
-        <v>-1.3</v>
+        <v>7.2</v>
+      </c>
+      <c r="I10" s="23">
+        <v>-2.2000000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>198</v>
+        <v>268</v>
       </c>
       <c r="C11" t="s">
-        <v>199</v>
+        <v>269</v>
       </c>
       <c r="D11" t="s">
-        <v>200</v>
+        <v>270</v>
       </c>
       <c r="E11" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="F11" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="G11">
-        <v>35.299999999999997</v>
+        <v>19.3</v>
       </c>
       <c r="H11">
-        <v>33.700000000000003</v>
+        <v>18.8</v>
       </c>
       <c r="I11">
-        <v>-1.5999999999999901</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G12" s="11">
-        <f>SUM(G9:G11)</f>
-        <v>100</v>
-      </c>
-      <c r="H12" s="11">
-        <f>SUM(H9:H11)</f>
-        <v>100.10000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="E13" s="21">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="F13" s="19">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="G13" s="18">
-        <v>36.1</v>
-      </c>
-      <c r="H13" s="18">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="I13" s="18">
-        <v>0.19999999999999599</v>
+      <c r="B12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C12" t="s">
+        <v>272</v>
+      </c>
+      <c r="D12" t="s">
+        <v>273</v>
+      </c>
+      <c r="E12" t="s">
+        <v>240</v>
+      </c>
+      <c r="F12" t="s">
+        <v>240</v>
+      </c>
+      <c r="G12">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="H12">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="I12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>274</v>
+      </c>
+      <c r="C13" t="s">
+        <v>275</v>
+      </c>
+      <c r="D13" t="s">
+        <v>276</v>
+      </c>
+      <c r="E13" t="s">
+        <v>240</v>
+      </c>
+      <c r="F13" t="s">
+        <v>240</v>
+      </c>
+      <c r="G13">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="H13">
+        <v>43.1</v>
+      </c>
+      <c r="I13" s="23">
+        <v>3.8</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>195</v>
+        <v>277</v>
       </c>
       <c r="C14" t="s">
-        <v>203</v>
+        <v>278</v>
       </c>
       <c r="D14" t="s">
-        <v>204</v>
+        <v>279</v>
       </c>
       <c r="E14" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="F14" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="G14">
-        <v>39.6</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="H14">
-        <v>40.799999999999997</v>
+        <v>11.3</v>
       </c>
       <c r="I14">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>198</v>
-      </c>
-      <c r="C15" t="s">
-        <v>205</v>
-      </c>
-      <c r="D15" t="s">
-        <v>206</v>
-      </c>
-      <c r="E15" t="s">
-        <v>166</v>
-      </c>
-      <c r="F15" t="s">
-        <v>166</v>
-      </c>
-      <c r="G15">
-        <v>24.4</v>
-      </c>
-      <c r="H15">
-        <v>23</v>
-      </c>
-      <c r="I15">
-        <v>-1.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G16" s="11">
-        <f>SUM(G13:G15)</f>
-        <v>100.1</v>
-      </c>
-      <c r="H16" s="11">
-        <f>SUM(H13:H15)</f>
-        <v>100.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="F17" s="23">
-        <v>0.37</v>
-      </c>
-      <c r="G17" s="18">
-        <v>56.8</v>
-      </c>
-      <c r="H17" s="18">
-        <v>74.099999999999994</v>
-      </c>
-      <c r="I17" s="24">
-        <v>17.3</v>
+      <c r="G15" s="3">
+        <f>SUM(G9:G14)</f>
+        <v>99.899999999999991</v>
+      </c>
+      <c r="H15" s="3">
+        <f>SUM(H9:H14)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="F16" s="21">
+        <v>0.254</v>
+      </c>
+      <c r="G16" s="18">
+        <v>11.8</v>
+      </c>
+      <c r="H16" s="18">
+        <v>6.4</v>
+      </c>
+      <c r="I16" s="22">
+        <v>-5.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C17" t="s">
+        <v>282</v>
+      </c>
+      <c r="D17" t="s">
+        <v>283</v>
+      </c>
+      <c r="E17" t="s">
+        <v>240</v>
+      </c>
+      <c r="F17" t="s">
+        <v>240</v>
+      </c>
+      <c r="G17">
+        <v>18.7</v>
+      </c>
+      <c r="H17">
+        <v>16.3</v>
+      </c>
+      <c r="I17">
+        <v>-2.4</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>210</v>
+        <v>268</v>
       </c>
       <c r="C18" t="s">
-        <v>211</v>
+        <v>284</v>
       </c>
       <c r="D18" t="s">
-        <v>212</v>
+        <v>285</v>
       </c>
       <c r="E18" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="F18" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="G18">
-        <v>43.2</v>
+        <v>29</v>
       </c>
       <c r="H18">
-        <v>25.9</v>
+        <v>27.7</v>
       </c>
       <c r="I18">
-        <v>-17.3</v>
+        <v>-1.3</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G19" s="11">
-        <f>SUM(G17:G18)</f>
-        <v>100</v>
-      </c>
-      <c r="H19" s="11">
-        <f>SUM(H17:H18)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>238</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="F20" s="23">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="G20" s="18">
-        <v>54.6</v>
-      </c>
-      <c r="H20" s="18">
-        <v>75.7</v>
-      </c>
-      <c r="I20" s="24">
-        <v>21.1</v>
+      <c r="B19" t="s">
+        <v>271</v>
+      </c>
+      <c r="C19" t="s">
+        <v>286</v>
+      </c>
+      <c r="D19" t="s">
+        <v>287</v>
+      </c>
+      <c r="E19" t="s">
+        <v>240</v>
+      </c>
+      <c r="F19" t="s">
+        <v>240</v>
+      </c>
+      <c r="G19">
+        <v>18.7</v>
+      </c>
+      <c r="H19">
+        <v>19.5</v>
+      </c>
+      <c r="I19">
+        <v>0.80000000000000104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>274</v>
+      </c>
+      <c r="C20" t="s">
+        <v>288</v>
+      </c>
+      <c r="D20" t="s">
+        <v>289</v>
+      </c>
+      <c r="E20" t="s">
+        <v>240</v>
+      </c>
+      <c r="F20" t="s">
+        <v>240</v>
+      </c>
+      <c r="G20">
+        <v>19</v>
+      </c>
+      <c r="H20">
+        <v>26.9</v>
+      </c>
+      <c r="I20" s="23">
+        <v>7.9</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>216</v>
+        <v>277</v>
       </c>
       <c r="C21" t="s">
-        <v>217</v>
+        <v>290</v>
       </c>
       <c r="D21" t="s">
-        <v>218</v>
+        <v>291</v>
       </c>
       <c r="E21" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="F21" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="G21">
-        <v>45.4</v>
+        <v>2.8</v>
       </c>
       <c r="H21">
-        <v>24.3</v>
+        <v>3.2</v>
       </c>
       <c r="I21">
-        <v>-21.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G22" s="11">
-        <f>SUM(G20:G21)</f>
-        <v>100</v>
-      </c>
-      <c r="H22" s="11">
-        <f>SUM(H20:H21)</f>
-        <v>100</v>
+      <c r="G22" s="3">
+        <f>SUM(G16:G21)</f>
+        <v>100</v>
+      </c>
+      <c r="H22" s="3">
+        <f>SUM(H16:H21)</f>
+        <v>100.00000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>239</v>
+        <v>318</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>219</v>
+        <v>262</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>220</v>
+        <v>292</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="F23" s="23">
-        <v>0.30499999999999999</v>
+        <v>293</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="F23" s="21">
+        <v>0.217</v>
       </c>
       <c r="G23" s="18">
-        <v>2.9</v>
+        <v>46</v>
       </c>
       <c r="H23" s="18">
-        <v>7</v>
-      </c>
-      <c r="I23" s="18">
-        <v>4.0999999999999996</v>
+        <v>36.299999999999997</v>
+      </c>
+      <c r="I23" s="22">
+        <v>-9.6999999999999993</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>222</v>
+        <v>265</v>
       </c>
       <c r="C24" t="s">
-        <v>223</v>
+        <v>294</v>
       </c>
       <c r="D24" t="s">
-        <v>224</v>
+        <v>295</v>
       </c>
       <c r="E24" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="F24" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="G24">
-        <v>18.3</v>
+        <v>29</v>
       </c>
       <c r="H24">
-        <v>21.8</v>
+        <v>32.1</v>
       </c>
       <c r="I24">
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>225</v>
+        <v>268</v>
       </c>
       <c r="C25" t="s">
-        <v>226</v>
+        <v>296</v>
       </c>
       <c r="D25" t="s">
-        <v>227</v>
+        <v>297</v>
       </c>
       <c r="E25" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="F25" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="G25">
-        <v>28.8</v>
+        <v>18</v>
       </c>
       <c r="H25">
-        <v>22.1</v>
-      </c>
-      <c r="I25" s="25">
-        <v>-6.7</v>
+        <v>20.7</v>
+      </c>
+      <c r="I25">
+        <v>2.7</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>228</v>
+        <v>271</v>
       </c>
       <c r="C26" t="s">
-        <v>229</v>
+        <v>298</v>
       </c>
       <c r="D26" t="s">
-        <v>230</v>
+        <v>299</v>
       </c>
       <c r="E26" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="F26" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="G26">
-        <v>26.7</v>
+        <v>4</v>
       </c>
       <c r="H26">
-        <v>32.5</v>
+        <v>5.9</v>
       </c>
       <c r="I26">
-        <v>5.8</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>231</v>
+        <v>274</v>
       </c>
       <c r="C27" t="s">
-        <v>232</v>
+        <v>300</v>
       </c>
       <c r="D27" t="s">
-        <v>233</v>
+        <v>301</v>
       </c>
       <c r="E27" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="F27" t="s">
-        <v>166</v>
+        <v>240</v>
       </c>
       <c r="G27">
-        <v>23.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H27">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="I27" s="25">
-        <v>-6.6</v>
+        <v>3.7</v>
+      </c>
+      <c r="I27">
+        <v>1.5</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G28" s="11">
-        <f>SUM(G23:G27)</f>
-        <v>99.9</v>
-      </c>
-      <c r="H28" s="11">
-        <f>SUM(H23:H27)</f>
-        <v>100</v>
+      <c r="B28" t="s">
+        <v>277</v>
+      </c>
+      <c r="C28" t="s">
+        <v>302</v>
+      </c>
+      <c r="D28" t="s">
+        <v>303</v>
+      </c>
+      <c r="E28" t="s">
+        <v>240</v>
+      </c>
+      <c r="F28" t="s">
+        <v>240</v>
+      </c>
+      <c r="G28">
+        <v>0.9</v>
+      </c>
+      <c r="H28">
+        <v>1.4</v>
+      </c>
+      <c r="I28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G29" s="3">
+        <f>SUM(G23:G28)</f>
+        <v>100.10000000000001</v>
+      </c>
+      <c r="H29" s="3">
+        <f>SUM(H23:H28)</f>
+        <v>100.10000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="F30" s="21">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="G30" s="18">
+        <v>50.4</v>
+      </c>
+      <c r="H30" s="18">
+        <v>47.3</v>
+      </c>
+      <c r="I30" s="22">
+        <v>-3.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>265</v>
+      </c>
+      <c r="C31" t="s">
+        <v>306</v>
+      </c>
+      <c r="D31" t="s">
+        <v>307</v>
+      </c>
+      <c r="E31" t="s">
+        <v>240</v>
+      </c>
+      <c r="F31" t="s">
+        <v>240</v>
+      </c>
+      <c r="G31">
+        <v>20</v>
+      </c>
+      <c r="H31">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="I31">
+        <v>-2.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>268</v>
+      </c>
+      <c r="C32" t="s">
+        <v>308</v>
+      </c>
+      <c r="D32" t="s">
+        <v>309</v>
+      </c>
+      <c r="E32" t="s">
+        <v>240</v>
+      </c>
+      <c r="F32" t="s">
+        <v>240</v>
+      </c>
+      <c r="G32">
+        <v>20.7</v>
+      </c>
+      <c r="H32">
+        <v>19.5</v>
+      </c>
+      <c r="I32">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>274</v>
+      </c>
+      <c r="C33" t="s">
+        <v>310</v>
+      </c>
+      <c r="D33" t="s">
+        <v>311</v>
+      </c>
+      <c r="E33" t="s">
+        <v>240</v>
+      </c>
+      <c r="F33" t="s">
+        <v>240</v>
+      </c>
+      <c r="G33">
+        <v>6.8</v>
+      </c>
+      <c r="H33">
+        <v>10</v>
+      </c>
+      <c r="I33" s="23">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>277</v>
+      </c>
+      <c r="C34" t="s">
+        <v>312</v>
+      </c>
+      <c r="D34" t="s">
+        <v>313</v>
+      </c>
+      <c r="E34" t="s">
+        <v>240</v>
+      </c>
+      <c r="F34" t="s">
+        <v>240</v>
+      </c>
+      <c r="G34">
+        <v>2.1</v>
+      </c>
+      <c r="H34">
+        <v>5.2</v>
+      </c>
+      <c r="I34" s="23">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G35" s="3">
+        <f>SUM(G30:G34)</f>
+        <v>100</v>
+      </c>
+      <c r="H35" s="3">
+        <f>SUM(H30:H34)</f>
+        <v>99.899999999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more descriptive stats on PROMs but with combined var cohort + comorb/demos
</commit_message>
<xml_diff>
--- a/summary_stats.xlsx
+++ b/summary_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m296398\Desktop\medicare_hos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998C2035-C4EB-46FD-9762-5249B2F3B873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D71D742-B259-4B7C-9FE1-4798578BA828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="315" windowWidth="14730" windowHeight="16155" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="315" windowWidth="14730" windowHeight="16155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="demos" sheetId="1" r:id="rId1"/>
@@ -1451,13 +1451,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
@@ -4774,7 +4774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>

</xml_diff>